<commit_message>
component engineering tracking folder
started a component engineering tracking folder. First document tracks
potential DVB ASICs.
</commit_message>
<xml_diff>
--- a/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
+++ b/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="1820" windowWidth="25600" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="4060" yWindow="920" windowWidth="25600" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
additional chips and visual differentiator added
</commit_message>
<xml_diff>
--- a/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
+++ b/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Si2167</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Website</t>
   </si>
   <si>
-    <t>modcods supported</t>
-  </si>
-  <si>
     <t>W6RZ successfully tested all of the 64800 bit MODCOD's (1 through 28 for DVB-S2 and 132 through 182 for DVB-S2X). No 16200 bit MODCOD's are supported (in either DVB-S2 or DVB-S2X). So the lowest SNR mode supported by the Si2169 is DVB-S2 QPSK 1/4 rate at -2.35 dB Es/No.</t>
   </si>
   <si>
@@ -49,6 +46,72 @@
   </si>
   <si>
     <t>best Es/No</t>
+  </si>
+  <si>
+    <t>discussion</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>http://www.electronicspecifier.com/communications/satellite-stb-supports-the-latest-dvb-s2x-broadcast-standard</t>
+  </si>
+  <si>
+    <t>Broadcom BCM453xx Series and BCM4501</t>
+  </si>
+  <si>
+    <t>MAX2112</t>
+  </si>
+  <si>
+    <t>https://www.maximintegrated.com/en/products/comms/wireless-rf/MAX2112.html</t>
+  </si>
+  <si>
+    <t>Not DVB-S2X, but could be used as a basis for an upper-end station that only uses 8PSK. The MAX2112 low-cost, direct-conversion tuner IC is designed for satellite set-top and VSAT applications. The IC is intended for 8PSK and Digital Video Broadcast (DVB-S2) applications.</t>
+  </si>
+  <si>
+    <t>MAX2121</t>
+  </si>
+  <si>
+    <t>Not DVB-S2X. Complete Direct-Conversion L-Band Tuner. The MAX2121 low-cost, direct-conversion tuner IC is designed for satellite set-top and VSAT applications. The device directly converts the satellite signals from the LNB to baseband using a broadband I/Q downconverter. The operating frequency range extends from 925MHz to 2175MHz.</t>
+  </si>
+  <si>
+    <t>https://www.maximintegrated.com/en/products/comms/wireless-rf/MAX2121.html</t>
+  </si>
+  <si>
+    <t>These chips might work</t>
+  </si>
+  <si>
+    <t>For comparison or variants</t>
+  </si>
+  <si>
+    <t>Section Headings Legend</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">250-2350 MHz spectrum is supported by this system-on-a-chip. Website claims all DVB-S2X modes supported. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Company extremely difficult to work with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Earlier version "Broadcom’s BCM4501 is a fully integrated dual satellite receiver single-chip solution targeted at multituner advanced modulation satellite receiver systems.
+The BCM4501 integrates dual CMOS tuners and dual advanced modulation decoders supporting DVB-S2 Broadcast and DVB-S applications. The highly integrated tuner sections are based on existing volume production technologies in Broadcom and on a direct conversion technology to reduce external components and increase performance. The product is suited for PVR-satellite receivers and integrated multifunction home media centers."</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -88,12 +151,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,22 +180,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,52 +549,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="68.1640625" customWidth="1"/>
-    <col min="3" max="3" width="56.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" ht="75">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="195">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="11" customFormat="1">
+      <c r="A10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="75">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E10" s="11" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Rumor Mill/Follow Up section
</commit_message>
<xml_diff>
--- a/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
+++ b/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Si2167</t>
   </si>
@@ -112,6 +112,69 @@
       <t>. Earlier version "Broadcom’s BCM4501 is a fully integrated dual satellite receiver single-chip solution targeted at multituner advanced modulation satellite receiver systems.
 The BCM4501 integrates dual CMOS tuners and dual advanced modulation decoders supporting DVB-S2 Broadcast and DVB-S applications. The highly integrated tuner sections are based on existing volume production technologies in Broadcom and on a direct conversion technology to reduce external components and increase performance. The product is suited for PVR-satellite receivers and integrated multifunction home media centers."</t>
     </r>
+  </si>
+  <si>
+    <t>STiD135</t>
+  </si>
+  <si>
+    <t>The STiD135 has been designed for Satellite Broadband applications, leveraging Ka-band and multi-spot beam technology carried by the latest high-throughput satellites (HTSs). The STiD135 has been designed to enable single-carrier usage of HTS transponders. The device implements two high-symbol-rate (HSR) demodulators compliant with Annex M of the DVB-S2/S2X specification EN 302 307, and provides full HW support for network clock recovery (NCR) in order to enable external return-channel modulators. The STiD135 may be used in standard broadcast environments as an 8-channel DVB-S2/S2X receiver enabling multi-channel distribution and/or fast channel change scenarios.</t>
+  </si>
+  <si>
+    <t>STiH332xCx</t>
+  </si>
+  <si>
+    <t>ARM Cortex-based, single-core, HEVC 1080p, DVB-S2/S2X set-top box SoC</t>
+  </si>
+  <si>
+    <t>http://www.st.com/content/st_com/en/products/digital-set-top-box-ics/hd-sd-set-top-box-processors/stih332xcx.html</t>
+  </si>
+  <si>
+    <t>http://www.st.com/content/st_com/en/products/digital-set-top-box-ics/demodulators-and-tuners/satellite-demodulators/stid135.html           http://www.st.com/content/ccc/resource/technical/document/data_brief/12/eb/69/e8/26/b0/4a/46/DM00136025.pdf/files/DM00136025.pdf/jcr:content/translations/en.DM00136025.pdf</t>
+  </si>
+  <si>
+    <t>AltoBeam</t>
+  </si>
+  <si>
+    <t>Creonic</t>
+  </si>
+  <si>
+    <t>AltoBeam, a leading demodulator chip supplier, has revealed that it is fully committed to S2X and the chip supporting S2X will be available early next year.</t>
+  </si>
+  <si>
+    <t>Creonic, an IP core provider that licenses the chip design to ASIC and FPGA implementers is currently working on an S2X design. They confirmed that the FEC part is ready and are now putting their efforts into the demodulator. They also note that with great interest in S2X, “some people are afraid that their competitors will support it and so they too will decide to implement it in order not to lose market share in the future”.</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>“we are currently engaged with several satellite operators and broadcasters to determine their requirements and their timing for the use of S2X for the DTH market. As this process is still ongoing we have not yet defined the specification or schedule for our DVB-S/S2/S2X IC development.</t>
+  </si>
+  <si>
+    <t>Teamcast</t>
+  </si>
+  <si>
+    <t>Long-time DVB contributor Teamcast has strongly supported the development and specification of DVB-S2X and its Vyper Satellite Modulator supports multiple standards including DVB-S, S2, and S2X.</t>
+  </si>
+  <si>
+    <t>DekTek</t>
+  </si>
+  <si>
+    <t>DekTec has a full implementation of DVB-S2X available now for its test modulator DTA-2115. It has in development an L-Band receiver card for PCI Express with support for DVB-S2X. This card is expected to be available in the market by the end of this year. DVB-S2X has been introduced at the same time as the new efficient HEVC video coding scheme. It is expected that new satellite receivers will combine these two technologies to make the delivery of HD and especially UHD services more efficient.</t>
+  </si>
+  <si>
+    <t>Work Microwave</t>
+  </si>
+  <si>
+    <t>Work Microwave plans to implement DVB-S2X for both their Broadcast Modulator SDM2, and professional IP Modem, SK-IP. The company will also introduce DVB-S2X products at IBC in September. These two device families make use of the broadcast profile and the professional profile.</t>
+  </si>
+  <si>
+    <t>AHA/Comtech</t>
+  </si>
+  <si>
+    <t>Follow up these rumors</t>
+  </si>
+  <si>
+    <t>DVB modem coming soon, announced at GNU Radio Conference, several kilobucks. Comtech EF Data have said “Our commitment to the broadcast community is to offer the products in a timeline that makes sense with the overall community.  We have indicated to our customers that we will support DVB-S2X and we will do this in conjunction with the availability of consumer and commercial IRDs”.</t>
   </si>
 </sst>
 </file>
@@ -151,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +233,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -180,14 +249,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -214,10 +284,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -581,6 +659,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="7" spans="1:5" s="8" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>2</v>
@@ -681,6 +764,101 @@
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="165">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="14" customFormat="1">
+      <c r="A17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="105">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="75">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="60">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="120">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="75">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="90">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added IBC2016 work microwave announcement
</commit_message>
<xml_diff>
--- a/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
+++ b/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Si2167</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Work Microwave</t>
   </si>
   <si>
-    <t>Work Microwave plans to implement DVB-S2X for both their Broadcast Modulator SDM2, and professional IP Modem, SK-IP. The company will also introduce DVB-S2X products at IBC in September. These two device families make use of the broadcast profile and the professional profile.</t>
-  </si>
-  <si>
     <t>AHA/Comtech</t>
   </si>
   <si>
@@ -175,6 +172,12 @@
   </si>
   <si>
     <t>DVB modem coming soon, announced at GNU Radio Conference, several kilobucks. Comtech EF Data have said “Our commitment to the broadcast community is to offer the products in a timeline that makes sense with the overall community.  We have indicated to our customers that we will support DVB-S2X and we will do this in conjunction with the availability of consumer and commercial IRDs”.</t>
+  </si>
+  <si>
+    <t>Work Microwave plans to implement DVB-S2X for both their Broadcast Modulator SDM2, and professional IP Modem, SK-IP. The company will also introduce DVB-S2X products at IBC in September. These two device families make use of the broadcast profile and the professional profile.    HOLZKIRCHEN, Germany — Sept. 20, 2016 — WORK Microwave, a leading European manufacturer of advanced satellite communications equipment, today announced a new single-carrier Wideband Demodulator that, when combined with the company’s Broadcast Modulator, provides satellite operators with one of the first end-to-end wideband transmission and reception solutions. Single-carrier operation mode for the Wideband Broadcast Modulator and Demodulator is based on the DVB-S2X standard, allowing the most efficient statistical multiplexing of different services and transmission over high-throughput satellite transponders with guaranteed power efficiency. Ideal for next-generation, high-speed IP-based broadcast and broadband access applications in Ka-, Ku-, Q-, and V-band satellite systems, WORK Microwave’s end-to-end wideband solution enables symbol rates of up to 500Msps.   WORK Microwave displayed a prototype of the Wideband Demodulator at IBC2016, with commercial availability in Q2 2017. The DVB-S2X Wideband Broadcast Modulator is now shipping.</t>
+  </si>
+  <si>
+    <t>https://work-microwave.com</t>
   </si>
 </sst>
 </file>
@@ -629,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -661,7 +664,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1">
@@ -845,20 +848,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="75">
+    <row r="29" spans="1:5" ht="330">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="90">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
very minor typo patrol
</commit_message>
<xml_diff>
--- a/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
+++ b/Manufacturing/Component_Engineering/DVB_ASICS_Phase_4_Ground.xlsx
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>